<commit_message>
data(li.ang): updated trading comments of HG1! in 2000.
</commit_message>
<xml_diff>
--- a/reviews/HG1!/2000/HG1!_2000_Review.xlsx
+++ b/reviews/HG1!/2000/HG1!_2000_Review.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="104">
   <si>
     <t>复盘编号</t>
   </si>
@@ -79,9 +79,6 @@
     <t>进场逻辑</t>
   </si>
   <si>
-    <t>评分</t>
-  </si>
-  <si>
     <t>进场信号</t>
   </si>
   <si>
@@ -94,6 +91,9 @@
     <t>仓位管理</t>
   </si>
   <si>
+    <t>总结</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
@@ -115,6 +115,66 @@
     <t>Short</t>
   </si>
   <si>
+    <t>盈利</t>
+  </si>
+  <si>
+    <t>反转：急速-通道-急速反转
+多头能量耗尽，做反转
+很好的入场逻辑</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">双K反转
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>信号K的反转力度不是很强</t>
+    </r>
+  </si>
+  <si>
+    <t>信号K上方一个Tick</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">通道下沿处止盈
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>下沿止盈部分仓位
+余下仓位移动止盈</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>优质交易</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+止盈太保守了</t>
+    </r>
+  </si>
+  <si>
     <t>头肩底</t>
   </si>
   <si>
@@ -124,34 +184,671 @@
     <t>Long</t>
   </si>
   <si>
+    <t>亏损</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">多次测试支撑位的反弹
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>此处是微型交易区间
+区间内的急速运动不应该入场</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">单根强势阳线
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>该阳线并未突破微型交易区间</t>
+    </r>
+  </si>
+  <si>
+    <t>价格密集区下方</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">前波段高点附近
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>前高点附近部分止盈
+余下仓位移动止盈</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>劣质交易</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+进场逻辑和进场信号都不充分</t>
+    </r>
+  </si>
+  <si>
     <t>突破</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">并没有什么好的逻辑
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>应当等待突破交易区间
+并且观察到明确的跟随</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">单根强势阳线
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>该阳线并未突破交易区间高点</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">信号K下方一个Tick
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>信号K体积过大
+盈亏比差</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>劣质交易</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+进场逻辑不充分
+进场信号体积太大</t>
+    </r>
+  </si>
+  <si>
     <t>区间</t>
   </si>
   <si>
     <t>Buy Limit</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">区间：高抛低吸
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>经过验证的通道</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>从概率的角度应该做空</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">无信号
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>应当等信号出现
+少做左侧交易</t>
+    </r>
+  </si>
+  <si>
+    <t>区间下沿宽止损</t>
+  </si>
+  <si>
+    <t>区间上沿1/3处止盈</t>
+  </si>
+  <si>
+    <r>
+      <t>一般交易</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+交易区间沿顺势方向做会更好</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">弱下跌趋势中的反弹
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>重叠的K线更像是交易区间</t>
+    </r>
+  </si>
+  <si>
+    <t>前波段高点附近</t>
+  </si>
+  <si>
+    <r>
+      <t>劣质交易</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+进场逻辑不充分
+进场信号并未大幅突破</t>
+    </r>
+  </si>
+  <si>
     <t>回调</t>
   </si>
   <si>
+    <t>趋势：简单调整</t>
+  </si>
+  <si>
+    <t>单根强势阳线</t>
+  </si>
+  <si>
+    <t>前波段高点上方一个Tick</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">固定盈亏比
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>达到目标盈亏比时部分止盈
+余下仓位移动止盈</t>
+    </r>
+  </si>
+  <si>
+    <t>优质交易</t>
+  </si>
+  <si>
     <t>三推楔形</t>
   </si>
   <si>
+    <t>反转：三推楔形</t>
+  </si>
+  <si>
+    <t>单根强势阴线</t>
+  </si>
+  <si>
+    <t>楔形高点</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">移动止盈
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>止盈太早
+并没有出现强势大阳线</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>优质交易</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+由于止盈原因比较可惜
+而且没有再次入场</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">通道：高抛低吸
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>赌突破失败
+未经验证的通道</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>劣质交易</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+未经验证的通道</t>
+    </r>
+  </si>
+  <si>
+    <t>趋势：旗形调整</t>
+  </si>
+  <si>
+    <t>前波段低点下方一个Tick</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">反转：直接反转
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>直接反转显然是小概率事件</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">单根强势阴线
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>此处为宽通道中的强势阴线
+且在EMA20处，应当多观察</t>
+    </r>
+  </si>
+  <si>
+    <t>回补缺口</t>
+  </si>
+  <si>
+    <r>
+      <t>劣质交易</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+应该按牛旗的形态做
+这笔交易完全不知道在干嘛</t>
+    </r>
+  </si>
+  <si>
     <t>MTP</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">趋势：突破追涨
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>高开强势突破</t>
+    </r>
+  </si>
+  <si>
+    <t>缺口下方一个Tick</t>
+  </si>
+  <si>
+    <t>移动止盈</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">趋势：简单调整
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>需要突破前高确认趋势延续</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>劣质交易</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+没确认趋势延续就入场</t>
+    </r>
+  </si>
+  <si>
+    <t>趋势：强势突破</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">信号K上方一个Tick
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>信号K体积过大
+盈亏比差</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">回补缺口
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>移动止盈更好</t>
+    </r>
+  </si>
+  <si>
     <t>楔形反转</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">反转：三推楔形
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>很好的入场逻辑</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">信号K下方一个Tick
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>止损设置的太紧
+应当设置为重要支撑位下方</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">楔形起点处
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>楔形起点处部分止盈
+余下仓位移动止盈</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>优质交易</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+由于止损原因比较可惜
+而且没有再次入场</t>
+    </r>
+  </si>
+  <si>
     <t>二段下跌</t>
   </si>
   <si>
     <t>Sell Limit</t>
   </si>
   <si>
-    <t>总结</t>
+    <r>
+      <t xml:space="preserve">趋势：简单调整
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>背景很差</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">单根强势阴线
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>信号K完全无法与背景K线相比</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">莫名其妙的止损点
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>信号K上方一个Tick就可以</t>
+    </r>
+  </si>
+  <si>
+    <t>前波段低点附近</t>
+  </si>
+  <si>
+    <r>
+      <t>劣质交易</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+背景很差
+信号K也很差</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -160,15 +857,15 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="8">
     <numFmt numFmtId="176" formatCode="0.0_ "/>
-    <numFmt numFmtId="177" formatCode="0.0000_ "/>
-    <numFmt numFmtId="178" formatCode="[$-409]yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="0_ "/>
-    <numFmt numFmtId="181" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="182" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="183" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="0.0000_ "/>
+    <numFmt numFmtId="180" formatCode="[$-409]yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="181" formatCode="0_ "/>
+    <numFmt numFmtId="182" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="183" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,22 +899,37 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="7"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -232,30 +944,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -269,16 +972,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -294,7 +989,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -303,21 +1013,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -339,7 +1034,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -354,37 +1072,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -402,19 +1120,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -426,7 +1174,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -438,43 +1228,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -486,60 +1246,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -598,27 +1316,56 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="medium">
+        <color auto="1"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -655,17 +1402,28 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -687,11 +1445,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -700,152 +1471,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -855,19 +1626,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -888,97 +1656,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="180" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -996,31 +1725,25 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1029,7 +1752,7 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1038,61 +1761,82 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1620,44 +2364,36 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AG17"/>
+  <dimension ref="A1:AU17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="Z26" sqref="Z26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72666666666667" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.90666666666667" style="4" customWidth="1"/>
-    <col min="2" max="2" width="11.82" style="5" customWidth="1"/>
-    <col min="3" max="5" width="9.90666666666667" style="6" customWidth="1"/>
-    <col min="6" max="6" width="9.90666666666667" style="4" customWidth="1"/>
-    <col min="7" max="7" width="11.82" style="5" customWidth="1"/>
-    <col min="8" max="8" width="9.90666666666667" style="6" customWidth="1"/>
-    <col min="9" max="9" width="10.6333333333333" style="6" customWidth="1"/>
-    <col min="10" max="10" width="9.90666666666667" style="6" customWidth="1"/>
-    <col min="11" max="12" width="11.82" style="7" customWidth="1"/>
-    <col min="13" max="13" width="9.90666666666667" style="8" customWidth="1"/>
-    <col min="14" max="14" width="11.82" style="5" customWidth="1"/>
-    <col min="15" max="15" width="11.82" style="7" customWidth="1"/>
-    <col min="16" max="16" width="9.90666666666667" style="9" customWidth="1"/>
-    <col min="17" max="17" width="8.09333333333333" style="10" customWidth="1"/>
-    <col min="18" max="19" width="12.2733333333333" style="11" customWidth="1"/>
-    <col min="20" max="20" width="7.54666666666667" style="12" customWidth="1"/>
-    <col min="21" max="21" width="19.6333333333333" style="13" customWidth="1"/>
-    <col min="22" max="22" width="5.72666666666667" style="13" customWidth="1"/>
-    <col min="23" max="23" width="20.82" style="13" customWidth="1"/>
-    <col min="24" max="24" width="5.72666666666667" style="13" customWidth="1"/>
-    <col min="25" max="25" width="14" style="13" customWidth="1"/>
-    <col min="26" max="26" width="5.72666666666667" style="13" customWidth="1"/>
-    <col min="27" max="27" width="16.2733333333333" style="13" customWidth="1"/>
-    <col min="28" max="28" width="5.72666666666667" style="13" customWidth="1"/>
-    <col min="29" max="29" width="23" style="13" customWidth="1"/>
-    <col min="30" max="30" width="5.72666666666667" style="13" customWidth="1"/>
-    <col min="31" max="16384" width="8.72666666666667" style="13"/>
+    <col min="1" max="1" width="7.7" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.4" style="4" customWidth="1"/>
+    <col min="3" max="5" width="7.7" style="5" customWidth="1"/>
+    <col min="6" max="6" width="7.7" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10.4" style="4" customWidth="1"/>
+    <col min="8" max="8" width="7.7" style="5" customWidth="1"/>
+    <col min="9" max="9" width="8.4" style="5" customWidth="1"/>
+    <col min="10" max="10" width="7.7" style="5" customWidth="1"/>
+    <col min="11" max="12" width="7.7" style="6" customWidth="1"/>
+    <col min="13" max="13" width="7.7" style="7" customWidth="1"/>
+    <col min="14" max="14" width="10.4" style="4" customWidth="1"/>
+    <col min="15" max="15" width="7.7" style="6" customWidth="1"/>
+    <col min="16" max="16" width="7.7" style="8" customWidth="1"/>
+    <col min="17" max="17" width="8" style="9" customWidth="1"/>
+    <col min="18" max="19" width="9.3" style="10" customWidth="1"/>
+    <col min="20" max="20" width="7.4" style="11" customWidth="1"/>
+    <col min="21" max="25" width="20.7" style="12" customWidth="1"/>
+    <col min="26" max="26" width="20.7" style="13" customWidth="1"/>
+    <col min="27" max="16384" width="8.72666666666667" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="15.75" spans="1:33">
+    <row r="1" s="1" customFormat="1" ht="15.75" spans="1:47">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1688,71 +2424,77 @@
       <c r="J1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="38" t="s">
+      <c r="K1" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="39" t="s">
+      <c r="L1" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="45" t="s">
+      <c r="M1" s="31" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="39" t="s">
+      <c r="O1" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="45" t="s">
+      <c r="P1" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="54" t="s">
+      <c r="Q1" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="55" t="s">
+      <c r="R1" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="55" t="s">
+      <c r="S1" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="54" t="s">
+      <c r="T1" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="72" t="s">
+      <c r="U1" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="72" t="s">
+      <c r="V1" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="72" t="s">
+      <c r="W1" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="72" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y1" s="72" t="s">
+      <c r="X1" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="72" t="s">
-        <v>21</v>
-      </c>
-      <c r="AA1" s="72" t="s">
+      <c r="Y1" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="72" t="s">
-        <v>21</v>
-      </c>
-      <c r="AC1" s="72" t="s">
+      <c r="Z1" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="AD1" s="72" t="s">
-        <v>21</v>
-      </c>
-      <c r="AE1" s="78"/>
-      <c r="AF1" s="79"/>
-      <c r="AG1" s="79"/>
+      <c r="AA1" s="62"/>
+      <c r="AB1" s="62"/>
+      <c r="AC1" s="62"/>
+      <c r="AD1" s="62"/>
+      <c r="AE1" s="62"/>
+      <c r="AF1" s="62"/>
+      <c r="AG1" s="62"/>
+      <c r="AH1" s="62"/>
+      <c r="AI1" s="62"/>
+      <c r="AJ1" s="62"/>
+      <c r="AK1" s="62"/>
+      <c r="AL1" s="62"/>
+      <c r="AM1" s="62"/>
+      <c r="AN1" s="62"/>
+      <c r="AO1" s="62"/>
+      <c r="AP1" s="62"/>
+      <c r="AQ1" s="62"/>
+      <c r="AR1" s="62"/>
+      <c r="AS1" s="62"/>
+      <c r="AT1" s="62"/>
+      <c r="AU1" s="62"/>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" ht="49.5" spans="1:47">
       <c r="A2" s="17" t="s">
         <v>26</v>
       </c>
@@ -1768,442 +2510,624 @@
       <c r="E2" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="26">
+      <c r="F2" s="17">
         <v>1</v>
       </c>
-      <c r="G2" s="27">
+      <c r="G2" s="18">
         <v>36546</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="40">
+      <c r="K2" s="28">
         <v>0.872</v>
       </c>
-      <c r="L2" s="40">
+      <c r="L2" s="28">
         <v>0.8865</v>
       </c>
-      <c r="M2" s="46">
+      <c r="M2" s="32">
         <v>1</v>
       </c>
-      <c r="N2" s="27">
+      <c r="N2" s="18">
         <v>36549</v>
       </c>
-      <c r="O2" s="40">
+      <c r="O2" s="28">
         <v>0.8565</v>
       </c>
-      <c r="P2" s="47">
+      <c r="P2" s="33">
         <v>1</v>
       </c>
-      <c r="Q2" s="56">
+      <c r="Q2" s="39">
         <v>0.0168</v>
       </c>
-      <c r="R2" s="57">
+      <c r="R2" s="40">
         <v>1.1</v>
       </c>
-      <c r="S2" s="57">
+      <c r="S2" s="41">
         <v>1.1</v>
       </c>
-      <c r="T2" s="58"/>
-      <c r="U2" s="73"/>
-      <c r="V2" s="73"/>
-      <c r="W2" s="73"/>
-      <c r="X2" s="73"/>
-      <c r="Y2" s="73"/>
-      <c r="Z2" s="73"/>
-      <c r="AA2" s="73"/>
-      <c r="AB2" s="73"/>
-      <c r="AC2" s="73"/>
-      <c r="AD2" s="73"/>
-      <c r="AE2" s="80"/>
-      <c r="AF2" s="80"/>
-      <c r="AG2" s="80"/>
+      <c r="T2" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="U2" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="V2" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="W2" s="55" t="s">
+        <v>36</v>
+      </c>
+      <c r="X2" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y2" s="55"/>
+      <c r="Z2" s="63" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA2" s="64"/>
+      <c r="AB2" s="64"/>
+      <c r="AC2" s="72"/>
+      <c r="AD2" s="72"/>
+      <c r="AE2" s="72"/>
+      <c r="AF2" s="72"/>
+      <c r="AG2" s="72"/>
+      <c r="AH2" s="72"/>
+      <c r="AI2" s="72"/>
+      <c r="AJ2" s="72"/>
+      <c r="AK2" s="72"/>
+      <c r="AL2" s="72"/>
+      <c r="AM2" s="72"/>
+      <c r="AN2" s="72"/>
+      <c r="AO2" s="72"/>
+      <c r="AP2" s="72"/>
+      <c r="AQ2" s="72"/>
+      <c r="AR2" s="72"/>
+      <c r="AS2" s="72"/>
+      <c r="AT2" s="72"/>
+      <c r="AU2" s="72"/>
     </row>
-    <row r="3" spans="1:33">
+    <row r="3" ht="49.5" spans="1:47">
       <c r="A3" s="20"/>
       <c r="B3" s="21"/>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
-      <c r="F3" s="29">
+      <c r="F3" s="20">
         <v>2</v>
       </c>
-      <c r="G3" s="30">
+      <c r="G3" s="21">
         <v>36557</v>
       </c>
-      <c r="H3" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="K3" s="41">
+      <c r="H3" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" s="29">
         <v>0.851</v>
       </c>
-      <c r="L3" s="41">
+      <c r="L3" s="29">
         <v>0.8305</v>
       </c>
-      <c r="M3" s="48">
+      <c r="M3" s="34">
         <v>1</v>
       </c>
-      <c r="N3" s="30">
+      <c r="N3" s="21">
         <v>36558</v>
       </c>
-      <c r="O3" s="41">
+      <c r="O3" s="29">
         <v>0.8305</v>
       </c>
-      <c r="P3" s="49">
+      <c r="P3" s="35">
         <v>1</v>
       </c>
-      <c r="Q3" s="59">
+      <c r="Q3" s="43">
         <v>0.0251</v>
       </c>
-      <c r="R3" s="60">
+      <c r="R3" s="44">
         <v>1.1</v>
       </c>
-      <c r="S3" s="60">
+      <c r="S3" s="45">
         <v>-1</v>
       </c>
-      <c r="T3" s="61"/>
-      <c r="U3" s="74"/>
-      <c r="V3" s="74"/>
-      <c r="W3" s="74"/>
-      <c r="X3" s="74"/>
-      <c r="Y3" s="74"/>
-      <c r="Z3" s="74"/>
-      <c r="AA3" s="74"/>
-      <c r="AB3" s="74"/>
-      <c r="AC3" s="74"/>
-      <c r="AD3" s="74"/>
-      <c r="AE3" s="80"/>
-      <c r="AF3" s="80"/>
-      <c r="AG3" s="80"/>
+      <c r="T3" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="U3" s="56" t="s">
+        <v>43</v>
+      </c>
+      <c r="V3" s="57" t="s">
+        <v>44</v>
+      </c>
+      <c r="W3" s="58" t="s">
+        <v>45</v>
+      </c>
+      <c r="X3" s="57" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y3" s="58"/>
+      <c r="Z3" s="65" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA3" s="64"/>
+      <c r="AB3" s="64"/>
+      <c r="AC3" s="72"/>
+      <c r="AD3" s="72"/>
+      <c r="AE3" s="72"/>
+      <c r="AF3" s="72"/>
+      <c r="AG3" s="72"/>
+      <c r="AH3" s="72"/>
+      <c r="AI3" s="72"/>
+      <c r="AJ3" s="72"/>
+      <c r="AK3" s="72"/>
+      <c r="AL3" s="72"/>
+      <c r="AM3" s="72"/>
+      <c r="AN3" s="72"/>
+      <c r="AO3" s="72"/>
+      <c r="AP3" s="72"/>
+      <c r="AQ3" s="72"/>
+      <c r="AR3" s="72"/>
+      <c r="AS3" s="72"/>
+      <c r="AT3" s="72"/>
+      <c r="AU3" s="72"/>
     </row>
-    <row r="4" spans="1:33">
+    <row r="4" ht="49.5" spans="1:47">
       <c r="A4" s="20"/>
       <c r="B4" s="21"/>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
       <c r="E4" s="22"/>
-      <c r="F4" s="29">
+      <c r="F4" s="20">
         <v>3</v>
       </c>
-      <c r="G4" s="30">
+      <c r="G4" s="21">
         <v>36567</v>
       </c>
-      <c r="H4" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="J4" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="K4" s="41">
+      <c r="H4" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" s="29">
         <v>0.853</v>
       </c>
-      <c r="L4" s="41">
+      <c r="L4" s="29">
         <v>0.827</v>
       </c>
-      <c r="M4" s="48">
+      <c r="M4" s="34">
         <v>1</v>
       </c>
-      <c r="N4" s="30">
+      <c r="N4" s="21">
         <v>36571</v>
       </c>
-      <c r="O4" s="41">
+      <c r="O4" s="29">
         <v>0.853</v>
       </c>
-      <c r="P4" s="49">
+      <c r="P4" s="35">
         <v>1</v>
       </c>
-      <c r="Q4" s="59">
+      <c r="Q4" s="43">
         <v>0.0315</v>
       </c>
-      <c r="R4" s="60">
+      <c r="R4" s="44">
         <v>0.8</v>
       </c>
-      <c r="S4" s="60">
+      <c r="S4" s="45">
         <v>-1</v>
       </c>
-      <c r="T4" s="61"/>
-      <c r="U4" s="74"/>
-      <c r="V4" s="74"/>
-      <c r="W4" s="74"/>
-      <c r="X4" s="74"/>
-      <c r="Y4" s="74"/>
-      <c r="Z4" s="74"/>
-      <c r="AA4" s="74"/>
-      <c r="AB4" s="74"/>
-      <c r="AC4" s="74"/>
-      <c r="AD4" s="74"/>
-      <c r="AE4" s="80"/>
-      <c r="AF4" s="80"/>
-      <c r="AG4" s="80"/>
+      <c r="T4" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="U4" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="V4" s="57" t="s">
+        <v>50</v>
+      </c>
+      <c r="W4" s="57" t="s">
+        <v>51</v>
+      </c>
+      <c r="X4" s="57" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y4" s="58"/>
+      <c r="Z4" s="65" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA4" s="64"/>
+      <c r="AB4" s="64"/>
+      <c r="AC4" s="72"/>
+      <c r="AD4" s="72"/>
+      <c r="AE4" s="72"/>
+      <c r="AF4" s="72"/>
+      <c r="AG4" s="72"/>
+      <c r="AH4" s="72"/>
+      <c r="AI4" s="72"/>
+      <c r="AJ4" s="72"/>
+      <c r="AK4" s="72"/>
+      <c r="AL4" s="72"/>
+      <c r="AM4" s="72"/>
+      <c r="AN4" s="72"/>
+      <c r="AO4" s="72"/>
+      <c r="AP4" s="72"/>
+      <c r="AQ4" s="72"/>
+      <c r="AR4" s="72"/>
+      <c r="AS4" s="72"/>
+      <c r="AT4" s="72"/>
+      <c r="AU4" s="72"/>
     </row>
-    <row r="5" spans="1:33">
+    <row r="5" ht="49.5" spans="1:47">
       <c r="A5" s="20"/>
       <c r="B5" s="21"/>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
-      <c r="F5" s="29">
+      <c r="F5" s="20">
         <v>4</v>
       </c>
-      <c r="G5" s="30">
+      <c r="G5" s="21">
         <v>36581</v>
       </c>
-      <c r="H5" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="I5" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="J5" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" s="41">
+      <c r="H5" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="J5" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="29">
         <v>0.8175</v>
       </c>
-      <c r="L5" s="41">
+      <c r="L5" s="29">
         <v>0.7935</v>
       </c>
-      <c r="M5" s="48">
+      <c r="M5" s="34">
         <v>1</v>
       </c>
-      <c r="N5" s="30">
+      <c r="N5" s="21">
         <v>36584</v>
       </c>
-      <c r="O5" s="41">
+      <c r="O5" s="29">
         <v>0.7935</v>
       </c>
-      <c r="P5" s="49">
+      <c r="P5" s="35">
         <v>1</v>
       </c>
-      <c r="Q5" s="59">
+      <c r="Q5" s="43">
         <v>0.0304</v>
       </c>
-      <c r="R5" s="60">
+      <c r="R5" s="44">
         <v>1.1</v>
       </c>
-      <c r="S5" s="60">
+      <c r="S5" s="45">
         <v>-1</v>
       </c>
-      <c r="T5" s="61"/>
-      <c r="U5" s="74"/>
-      <c r="V5" s="74"/>
-      <c r="W5" s="74"/>
-      <c r="X5" s="74"/>
-      <c r="Y5" s="74"/>
-      <c r="Z5" s="74"/>
-      <c r="AA5" s="74"/>
-      <c r="AB5" s="74"/>
-      <c r="AC5" s="74"/>
-      <c r="AD5" s="74"/>
-      <c r="AE5" s="80"/>
-      <c r="AF5" s="80"/>
-      <c r="AG5" s="80"/>
+      <c r="T5" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="U5" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="V5" s="57" t="s">
+        <v>56</v>
+      </c>
+      <c r="W5" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="X5" s="58" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y5" s="58"/>
+      <c r="Z5" s="66" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA5" s="64"/>
+      <c r="AB5" s="64"/>
+      <c r="AC5" s="72"/>
+      <c r="AD5" s="72"/>
+      <c r="AE5" s="72"/>
+      <c r="AF5" s="72"/>
+      <c r="AG5" s="72"/>
+      <c r="AH5" s="72"/>
+      <c r="AI5" s="72"/>
+      <c r="AJ5" s="72"/>
+      <c r="AK5" s="72"/>
+      <c r="AL5" s="72"/>
+      <c r="AM5" s="72"/>
+      <c r="AN5" s="72"/>
+      <c r="AO5" s="72"/>
+      <c r="AP5" s="72"/>
+      <c r="AQ5" s="72"/>
+      <c r="AR5" s="72"/>
+      <c r="AS5" s="72"/>
+      <c r="AT5" s="72"/>
+      <c r="AU5" s="72"/>
     </row>
-    <row r="6" spans="1:33">
+    <row r="6" ht="49.5" spans="1:47">
       <c r="A6" s="20"/>
       <c r="B6" s="21"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
-      <c r="F6" s="29">
+      <c r="F6" s="20">
         <v>5</v>
       </c>
-      <c r="G6" s="30">
+      <c r="G6" s="21">
         <v>36607</v>
       </c>
-      <c r="H6" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="I6" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="K6" s="41">
+      <c r="H6" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="29">
         <v>0.8225</v>
       </c>
-      <c r="L6" s="41">
+      <c r="L6" s="29">
         <v>0.804</v>
       </c>
-      <c r="M6" s="48">
+      <c r="M6" s="34">
         <v>1</v>
       </c>
-      <c r="N6" s="30">
+      <c r="N6" s="21">
         <v>36612</v>
       </c>
-      <c r="O6" s="41">
+      <c r="O6" s="29">
         <v>0.804</v>
       </c>
-      <c r="P6" s="49">
+      <c r="P6" s="35">
         <v>1</v>
       </c>
-      <c r="Q6" s="59">
+      <c r="Q6" s="43">
         <v>0.0235</v>
       </c>
-      <c r="R6" s="60">
+      <c r="R6" s="44">
         <v>1.5</v>
       </c>
-      <c r="S6" s="60">
+      <c r="S6" s="45">
         <v>-1</v>
       </c>
-      <c r="T6" s="61"/>
-      <c r="U6" s="74"/>
-      <c r="V6" s="74"/>
-      <c r="W6" s="74"/>
-      <c r="X6" s="74"/>
-      <c r="Y6" s="74"/>
-      <c r="Z6" s="74"/>
-      <c r="AA6" s="74"/>
-      <c r="AB6" s="74"/>
-      <c r="AC6" s="74"/>
-      <c r="AD6" s="74"/>
-      <c r="AE6" s="80"/>
-      <c r="AF6" s="80"/>
-      <c r="AG6" s="80"/>
+      <c r="T6" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="U6" s="56" t="s">
+        <v>60</v>
+      </c>
+      <c r="V6" s="57" t="s">
+        <v>44</v>
+      </c>
+      <c r="W6" s="58" t="s">
+        <v>45</v>
+      </c>
+      <c r="X6" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y6" s="58"/>
+      <c r="Z6" s="65" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA6" s="64"/>
+      <c r="AB6" s="64"/>
+      <c r="AC6" s="72"/>
+      <c r="AD6" s="72"/>
+      <c r="AE6" s="72"/>
+      <c r="AF6" s="72"/>
+      <c r="AG6" s="72"/>
+      <c r="AH6" s="72"/>
+      <c r="AI6" s="72"/>
+      <c r="AJ6" s="72"/>
+      <c r="AK6" s="72"/>
+      <c r="AL6" s="72"/>
+      <c r="AM6" s="72"/>
+      <c r="AN6" s="72"/>
+      <c r="AO6" s="72"/>
+      <c r="AP6" s="72"/>
+      <c r="AQ6" s="72"/>
+      <c r="AR6" s="72"/>
+      <c r="AS6" s="72"/>
+      <c r="AT6" s="72"/>
+      <c r="AU6" s="72"/>
     </row>
-    <row r="7" spans="1:33">
+    <row r="7" ht="49.5" spans="1:47">
       <c r="A7" s="20"/>
       <c r="B7" s="21"/>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
-      <c r="F7" s="29">
+      <c r="F7" s="20">
         <v>6</v>
       </c>
-      <c r="G7" s="30">
+      <c r="G7" s="21">
         <v>36630</v>
       </c>
-      <c r="H7" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" s="31" t="s">
+      <c r="H7" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="I7" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="J7" s="31" t="s">
+      <c r="J7" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="41">
+      <c r="K7" s="29">
         <v>0.767</v>
       </c>
-      <c r="L7" s="41">
+      <c r="L7" s="29">
         <v>0.7845</v>
       </c>
-      <c r="M7" s="48">
+      <c r="M7" s="34">
         <v>1</v>
       </c>
-      <c r="N7" s="30">
+      <c r="N7" s="21">
         <v>36634</v>
       </c>
-      <c r="O7" s="41">
+      <c r="O7" s="29">
         <v>0.7495</v>
       </c>
-      <c r="P7" s="49">
+      <c r="P7" s="35">
         <v>1</v>
       </c>
-      <c r="Q7" s="62">
+      <c r="Q7" s="46">
         <v>0.0208</v>
       </c>
-      <c r="R7" s="60">
+      <c r="R7" s="44">
         <v>1</v>
       </c>
-      <c r="S7" s="60">
+      <c r="S7" s="45">
         <v>1</v>
       </c>
-      <c r="T7" s="61"/>
-      <c r="U7" s="74"/>
-      <c r="V7" s="74"/>
-      <c r="W7" s="74"/>
-      <c r="X7" s="74"/>
-      <c r="Y7" s="74"/>
-      <c r="Z7" s="74"/>
-      <c r="AA7" s="74"/>
-      <c r="AB7" s="74"/>
-      <c r="AC7" s="74"/>
-      <c r="AD7" s="74"/>
-      <c r="AE7" s="80"/>
-      <c r="AF7" s="80"/>
-      <c r="AG7" s="80"/>
+      <c r="T7" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="U7" s="59" t="s">
+        <v>64</v>
+      </c>
+      <c r="V7" s="58" t="s">
+        <v>65</v>
+      </c>
+      <c r="W7" s="58" t="s">
+        <v>66</v>
+      </c>
+      <c r="X7" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y7" s="58"/>
+      <c r="Z7" s="67" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA7" s="64"/>
+      <c r="AB7" s="64"/>
+      <c r="AC7" s="72"/>
+      <c r="AD7" s="72"/>
+      <c r="AE7" s="72"/>
+      <c r="AF7" s="72"/>
+      <c r="AG7" s="72"/>
+      <c r="AH7" s="72"/>
+      <c r="AI7" s="72"/>
+      <c r="AJ7" s="72"/>
+      <c r="AK7" s="72"/>
+      <c r="AL7" s="72"/>
+      <c r="AM7" s="72"/>
+      <c r="AN7" s="72"/>
+      <c r="AO7" s="72"/>
+      <c r="AP7" s="72"/>
+      <c r="AQ7" s="72"/>
+      <c r="AR7" s="72"/>
+      <c r="AS7" s="72"/>
+      <c r="AT7" s="72"/>
+      <c r="AU7" s="72"/>
     </row>
-    <row r="8" s="2" customFormat="1" spans="1:33">
+    <row r="8" s="2" customFormat="1" ht="49.5" spans="1:47">
       <c r="A8" s="20"/>
       <c r="B8" s="21"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
-      <c r="F8" s="32">
+      <c r="F8" s="23">
         <v>7</v>
       </c>
-      <c r="G8" s="33">
+      <c r="G8" s="24">
         <v>36665</v>
       </c>
-      <c r="H8" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="I8" s="34" t="s">
+      <c r="H8" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="I8" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="J8" s="34" t="s">
+      <c r="J8" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="42">
+      <c r="K8" s="30">
         <v>0.84</v>
       </c>
-      <c r="L8" s="42">
+      <c r="L8" s="30">
         <v>0.856</v>
       </c>
-      <c r="M8" s="49">
+      <c r="M8" s="35">
         <v>1</v>
       </c>
-      <c r="N8" s="33">
+      <c r="N8" s="24">
         <v>36669</v>
       </c>
-      <c r="O8" s="42">
+      <c r="O8" s="30">
         <v>0.8345</v>
       </c>
-      <c r="P8" s="49">
+      <c r="P8" s="35">
         <v>1</v>
       </c>
-      <c r="Q8" s="62">
+      <c r="Q8" s="46">
         <v>0.0055</v>
       </c>
-      <c r="R8" s="63">
+      <c r="R8" s="47">
         <v>1.5</v>
       </c>
-      <c r="S8" s="63">
+      <c r="S8" s="48">
         <v>0.3</v>
       </c>
-      <c r="T8" s="64"/>
-      <c r="U8" s="75"/>
-      <c r="V8" s="75"/>
-      <c r="W8" s="75"/>
-      <c r="X8" s="75"/>
-      <c r="Y8" s="75"/>
-      <c r="Z8" s="75"/>
-      <c r="AA8" s="75"/>
-      <c r="AB8" s="75"/>
-      <c r="AC8" s="75"/>
-      <c r="AD8" s="75"/>
-      <c r="AE8" s="81"/>
-      <c r="AF8" s="81"/>
-      <c r="AG8" s="81"/>
+      <c r="T8" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="U8" s="60" t="s">
+        <v>70</v>
+      </c>
+      <c r="V8" s="61" t="s">
+        <v>71</v>
+      </c>
+      <c r="W8" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="X8" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y8" s="61"/>
+      <c r="Z8" s="68" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA8" s="69"/>
+      <c r="AB8" s="69"/>
+      <c r="AC8" s="73"/>
+      <c r="AD8" s="73"/>
+      <c r="AE8" s="73"/>
+      <c r="AF8" s="73"/>
+      <c r="AG8" s="73"/>
+      <c r="AH8" s="73"/>
+      <c r="AI8" s="73"/>
+      <c r="AJ8" s="73"/>
+      <c r="AK8" s="73"/>
+      <c r="AL8" s="73"/>
+      <c r="AM8" s="73"/>
+      <c r="AN8" s="73"/>
+      <c r="AO8" s="73"/>
+      <c r="AP8" s="73"/>
+      <c r="AQ8" s="73"/>
+      <c r="AR8" s="73"/>
+      <c r="AS8" s="73"/>
+      <c r="AT8" s="73"/>
+      <c r="AU8" s="73"/>
     </row>
-    <row r="9" spans="1:33">
+    <row r="9" ht="49.5" spans="1:47">
       <c r="A9" s="20"/>
       <c r="B9" s="21"/>
       <c r="C9" s="22"/>
@@ -2219,54 +3143,80 @@
         <v>30</v>
       </c>
       <c r="I9" s="22" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="J9" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="K9" s="43">
+        <v>41</v>
+      </c>
+      <c r="K9" s="29">
         <v>0.8355</v>
       </c>
-      <c r="L9" s="43">
+      <c r="L9" s="29">
         <v>0.813</v>
       </c>
-      <c r="M9" s="50">
+      <c r="M9" s="34">
         <v>1</v>
       </c>
       <c r="N9" s="21">
         <v>36676</v>
       </c>
-      <c r="O9" s="43">
+      <c r="O9" s="29">
         <v>0.813</v>
       </c>
-      <c r="P9" s="51">
+      <c r="P9" s="35">
         <v>1</v>
       </c>
-      <c r="Q9" s="65">
+      <c r="Q9" s="43">
         <v>0.0279</v>
       </c>
-      <c r="R9" s="66">
+      <c r="R9" s="44">
         <v>0.8</v>
       </c>
-      <c r="S9" s="66">
+      <c r="S9" s="45">
         <v>-1</v>
       </c>
-      <c r="T9" s="67"/>
-      <c r="U9" s="76"/>
-      <c r="V9" s="76"/>
-      <c r="W9" s="76"/>
-      <c r="X9" s="76"/>
-      <c r="Y9" s="76"/>
-      <c r="Z9" s="76"/>
-      <c r="AA9" s="76"/>
-      <c r="AB9" s="76"/>
-      <c r="AC9" s="76"/>
-      <c r="AD9" s="76"/>
-      <c r="AE9" s="80"/>
-      <c r="AF9" s="80"/>
-      <c r="AG9" s="80"/>
+      <c r="T9" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="U9" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="V9" s="57" t="s">
+        <v>56</v>
+      </c>
+      <c r="W9" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="X9" s="58" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y9" s="58"/>
+      <c r="Z9" s="65" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA9" s="64"/>
+      <c r="AB9" s="64"/>
+      <c r="AC9" s="72"/>
+      <c r="AD9" s="72"/>
+      <c r="AE9" s="72"/>
+      <c r="AF9" s="72"/>
+      <c r="AG9" s="72"/>
+      <c r="AH9" s="72"/>
+      <c r="AI9" s="72"/>
+      <c r="AJ9" s="72"/>
+      <c r="AK9" s="72"/>
+      <c r="AL9" s="72"/>
+      <c r="AM9" s="72"/>
+      <c r="AN9" s="72"/>
+      <c r="AO9" s="72"/>
+      <c r="AP9" s="72"/>
+      <c r="AQ9" s="72"/>
+      <c r="AR9" s="72"/>
+      <c r="AS9" s="72"/>
+      <c r="AT9" s="72"/>
+      <c r="AU9" s="72"/>
     </row>
-    <row r="10" spans="1:33">
+    <row r="10" ht="49.5" spans="1:47">
       <c r="A10" s="20"/>
       <c r="B10" s="21"/>
       <c r="C10" s="22"/>
@@ -2279,57 +3229,83 @@
         <v>36692</v>
       </c>
       <c r="H10" s="22" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="I10" s="22" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="J10" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="K10" s="43">
+        <v>41</v>
+      </c>
+      <c r="K10" s="29">
         <v>0.8125</v>
       </c>
-      <c r="L10" s="43">
+      <c r="L10" s="29">
         <v>0.784</v>
       </c>
-      <c r="M10" s="50">
+      <c r="M10" s="34">
         <v>1</v>
       </c>
       <c r="N10" s="21">
         <v>36699</v>
       </c>
-      <c r="O10" s="43">
+      <c r="O10" s="29">
         <v>0.8175</v>
       </c>
-      <c r="P10" s="51">
+      <c r="P10" s="35">
         <v>1</v>
       </c>
-      <c r="Q10" s="68">
+      <c r="Q10" s="46">
         <v>0.0052</v>
       </c>
-      <c r="R10" s="66">
+      <c r="R10" s="44">
         <v>1</v>
       </c>
-      <c r="S10" s="66">
+      <c r="S10" s="45">
         <v>0.2</v>
       </c>
-      <c r="T10" s="67"/>
-      <c r="U10" s="76"/>
-      <c r="V10" s="76"/>
-      <c r="W10" s="76"/>
-      <c r="X10" s="76"/>
-      <c r="Y10" s="76"/>
-      <c r="Z10" s="76"/>
-      <c r="AA10" s="76"/>
-      <c r="AB10" s="76"/>
-      <c r="AC10" s="76"/>
-      <c r="AD10" s="76"/>
-      <c r="AE10" s="80"/>
-      <c r="AF10" s="80"/>
-      <c r="AG10" s="80"/>
+      <c r="T10" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="U10" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="V10" s="58" t="s">
+        <v>65</v>
+      </c>
+      <c r="W10" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="X10" s="57" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y10" s="58"/>
+      <c r="Z10" s="68" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA10" s="64"/>
+      <c r="AB10" s="64"/>
+      <c r="AC10" s="72"/>
+      <c r="AD10" s="72"/>
+      <c r="AE10" s="72"/>
+      <c r="AF10" s="72"/>
+      <c r="AG10" s="72"/>
+      <c r="AH10" s="72"/>
+      <c r="AI10" s="72"/>
+      <c r="AJ10" s="72"/>
+      <c r="AK10" s="72"/>
+      <c r="AL10" s="72"/>
+      <c r="AM10" s="72"/>
+      <c r="AN10" s="72"/>
+      <c r="AO10" s="72"/>
+      <c r="AP10" s="72"/>
+      <c r="AQ10" s="72"/>
+      <c r="AR10" s="72"/>
+      <c r="AS10" s="72"/>
+      <c r="AT10" s="72"/>
+      <c r="AU10" s="72"/>
     </row>
-    <row r="11" spans="1:33">
+    <row r="11" ht="49.5" spans="1:47">
       <c r="A11" s="20"/>
       <c r="B11" s="21"/>
       <c r="C11" s="22"/>
@@ -2350,49 +3326,75 @@
       <c r="J11" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="K11" s="43">
+      <c r="K11" s="29">
         <v>0.858</v>
       </c>
-      <c r="L11" s="43">
+      <c r="L11" s="29">
         <v>0.883</v>
       </c>
-      <c r="M11" s="50">
+      <c r="M11" s="34">
         <v>1</v>
       </c>
       <c r="N11" s="21">
         <v>36768</v>
       </c>
-      <c r="O11" s="43">
+      <c r="O11" s="29">
         <v>0.883</v>
       </c>
-      <c r="P11" s="51">
+      <c r="P11" s="35">
         <v>1</v>
       </c>
-      <c r="Q11" s="65">
+      <c r="Q11" s="43">
         <v>0.0301</v>
       </c>
-      <c r="R11" s="66">
+      <c r="R11" s="44">
         <v>0.6</v>
       </c>
-      <c r="S11" s="66">
+      <c r="S11" s="45">
         <v>-1</v>
       </c>
-      <c r="T11" s="67"/>
-      <c r="U11" s="76"/>
-      <c r="V11" s="76"/>
-      <c r="W11" s="76"/>
-      <c r="X11" s="76"/>
-      <c r="Y11" s="76"/>
-      <c r="Z11" s="76"/>
-      <c r="AA11" s="76"/>
-      <c r="AB11" s="76"/>
-      <c r="AC11" s="76"/>
-      <c r="AD11" s="76"/>
-      <c r="AE11" s="80"/>
-      <c r="AF11" s="80"/>
-      <c r="AG11" s="80"/>
+      <c r="T11" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="U11" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="V11" s="57" t="s">
+        <v>80</v>
+      </c>
+      <c r="W11" s="58" t="s">
+        <v>66</v>
+      </c>
+      <c r="X11" s="58" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y11" s="58"/>
+      <c r="Z11" s="65" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA11" s="64"/>
+      <c r="AB11" s="64"/>
+      <c r="AC11" s="72"/>
+      <c r="AD11" s="72"/>
+      <c r="AE11" s="72"/>
+      <c r="AF11" s="72"/>
+      <c r="AG11" s="72"/>
+      <c r="AH11" s="72"/>
+      <c r="AI11" s="72"/>
+      <c r="AJ11" s="72"/>
+      <c r="AK11" s="72"/>
+      <c r="AL11" s="72"/>
+      <c r="AM11" s="72"/>
+      <c r="AN11" s="72"/>
+      <c r="AO11" s="72"/>
+      <c r="AP11" s="72"/>
+      <c r="AQ11" s="72"/>
+      <c r="AR11" s="72"/>
+      <c r="AS11" s="72"/>
+      <c r="AT11" s="72"/>
+      <c r="AU11" s="72"/>
     </row>
-    <row r="12" spans="1:33">
+    <row r="12" ht="33" spans="1:47">
       <c r="A12" s="20"/>
       <c r="B12" s="21"/>
       <c r="C12" s="22"/>
@@ -2405,57 +3407,83 @@
         <v>36769</v>
       </c>
       <c r="H12" s="22" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="I12" s="22" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="J12" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="K12" s="43">
+        <v>41</v>
+      </c>
+      <c r="K12" s="29">
         <v>0.8985</v>
       </c>
-      <c r="L12" s="43">
+      <c r="L12" s="29">
         <v>0.879</v>
       </c>
-      <c r="M12" s="50">
+      <c r="M12" s="34">
         <v>1</v>
       </c>
       <c r="N12" s="21">
         <v>36782</v>
       </c>
-      <c r="O12" s="43">
+      <c r="O12" s="29">
         <v>0.937</v>
       </c>
-      <c r="P12" s="51">
+      <c r="P12" s="35">
         <v>1</v>
       </c>
-      <c r="Q12" s="68">
+      <c r="Q12" s="46">
         <v>0.0418</v>
       </c>
-      <c r="R12" s="66" t="s">
-        <v>41</v>
-      </c>
-      <c r="S12" s="66">
+      <c r="R12" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="S12" s="45">
         <v>2</v>
       </c>
-      <c r="T12" s="67"/>
-      <c r="U12" s="76"/>
-      <c r="V12" s="76"/>
-      <c r="W12" s="76"/>
-      <c r="X12" s="76"/>
-      <c r="Y12" s="76"/>
-      <c r="Z12" s="76"/>
-      <c r="AA12" s="76"/>
-      <c r="AB12" s="76"/>
-      <c r="AC12" s="76"/>
-      <c r="AD12" s="76"/>
-      <c r="AE12" s="80"/>
-      <c r="AF12" s="80"/>
-      <c r="AG12" s="80"/>
+      <c r="T12" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="U12" s="56" t="s">
+        <v>84</v>
+      </c>
+      <c r="V12" s="58" t="s">
+        <v>65</v>
+      </c>
+      <c r="W12" s="58" t="s">
+        <v>85</v>
+      </c>
+      <c r="X12" s="58" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y12" s="58"/>
+      <c r="Z12" s="67" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA12" s="64"/>
+      <c r="AB12" s="64"/>
+      <c r="AC12" s="72"/>
+      <c r="AD12" s="72"/>
+      <c r="AE12" s="72"/>
+      <c r="AF12" s="72"/>
+      <c r="AG12" s="72"/>
+      <c r="AH12" s="72"/>
+      <c r="AI12" s="72"/>
+      <c r="AJ12" s="72"/>
+      <c r="AK12" s="72"/>
+      <c r="AL12" s="72"/>
+      <c r="AM12" s="72"/>
+      <c r="AN12" s="72"/>
+      <c r="AO12" s="72"/>
+      <c r="AP12" s="72"/>
+      <c r="AQ12" s="72"/>
+      <c r="AR12" s="72"/>
+      <c r="AS12" s="72"/>
+      <c r="AT12" s="72"/>
+      <c r="AU12" s="72"/>
     </row>
-    <row r="13" spans="1:33">
+    <row r="13" ht="49.5" spans="1:47">
       <c r="A13" s="20"/>
       <c r="B13" s="21"/>
       <c r="C13" s="22"/>
@@ -2468,57 +3496,83 @@
         <v>36791</v>
       </c>
       <c r="H13" s="22" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="I13" s="22" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="J13" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="K13" s="43">
+        <v>41</v>
+      </c>
+      <c r="K13" s="29">
         <v>0.9345</v>
       </c>
-      <c r="L13" s="43">
+      <c r="L13" s="29">
         <v>0.9055</v>
       </c>
-      <c r="M13" s="50">
+      <c r="M13" s="34">
         <v>1</v>
       </c>
       <c r="N13" s="21">
         <v>36801</v>
       </c>
-      <c r="O13" s="43">
+      <c r="O13" s="29">
         <v>0.9055</v>
       </c>
-      <c r="P13" s="51">
+      <c r="P13" s="35">
         <v>1</v>
       </c>
-      <c r="Q13" s="65">
+      <c r="Q13" s="43">
         <v>0.032</v>
       </c>
-      <c r="R13" s="66" t="s">
-        <v>41</v>
-      </c>
-      <c r="S13" s="66">
+      <c r="R13" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="S13" s="45">
         <v>-1</v>
       </c>
-      <c r="T13" s="67"/>
-      <c r="U13" s="76"/>
-      <c r="V13" s="76"/>
-      <c r="W13" s="76"/>
-      <c r="X13" s="76"/>
-      <c r="Y13" s="76"/>
-      <c r="Z13" s="76"/>
-      <c r="AA13" s="76"/>
-      <c r="AB13" s="76"/>
-      <c r="AC13" s="76"/>
-      <c r="AD13" s="76"/>
-      <c r="AE13" s="80"/>
-      <c r="AF13" s="80"/>
-      <c r="AG13" s="80"/>
+      <c r="T13" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="U13" s="56" t="s">
+        <v>87</v>
+      </c>
+      <c r="V13" s="57" t="s">
+        <v>50</v>
+      </c>
+      <c r="W13" s="57" t="s">
+        <v>51</v>
+      </c>
+      <c r="X13" s="58" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y13" s="58"/>
+      <c r="Z13" s="65" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA13" s="64"/>
+      <c r="AB13" s="64"/>
+      <c r="AC13" s="72"/>
+      <c r="AD13" s="72"/>
+      <c r="AE13" s="72"/>
+      <c r="AF13" s="72"/>
+      <c r="AG13" s="72"/>
+      <c r="AH13" s="72"/>
+      <c r="AI13" s="72"/>
+      <c r="AJ13" s="72"/>
+      <c r="AK13" s="72"/>
+      <c r="AL13" s="72"/>
+      <c r="AM13" s="72"/>
+      <c r="AN13" s="72"/>
+      <c r="AO13" s="72"/>
+      <c r="AP13" s="72"/>
+      <c r="AQ13" s="72"/>
+      <c r="AR13" s="72"/>
+      <c r="AS13" s="72"/>
+      <c r="AT13" s="72"/>
+      <c r="AU13" s="72"/>
     </row>
-    <row r="14" spans="1:33">
+    <row r="14" ht="49.5" spans="1:47">
       <c r="A14" s="20"/>
       <c r="B14" s="21"/>
       <c r="C14" s="22"/>
@@ -2531,7 +3585,7 @@
         <v>36812</v>
       </c>
       <c r="H14" s="22" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="I14" s="22" t="s">
         <v>31</v>
@@ -2539,49 +3593,75 @@
       <c r="J14" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="K14" s="43">
+      <c r="K14" s="29">
         <v>0.8805</v>
       </c>
-      <c r="L14" s="43">
+      <c r="L14" s="29">
         <v>0.9045</v>
       </c>
-      <c r="M14" s="50">
+      <c r="M14" s="34">
         <v>1</v>
       </c>
       <c r="N14" s="21">
         <v>36825</v>
       </c>
-      <c r="O14" s="43">
+      <c r="O14" s="29">
         <v>0.8465</v>
       </c>
-      <c r="P14" s="51">
+      <c r="P14" s="35">
         <v>1</v>
       </c>
-      <c r="Q14" s="68">
+      <c r="Q14" s="46">
         <v>0.0376</v>
       </c>
-      <c r="R14" s="66">
+      <c r="R14" s="44">
         <v>1.4</v>
       </c>
-      <c r="S14" s="66">
+      <c r="S14" s="45">
         <v>1.4</v>
       </c>
-      <c r="T14" s="67"/>
-      <c r="U14" s="76"/>
-      <c r="V14" s="76"/>
-      <c r="W14" s="76"/>
-      <c r="X14" s="76"/>
-      <c r="Y14" s="76"/>
-      <c r="Z14" s="76"/>
-      <c r="AA14" s="76"/>
-      <c r="AB14" s="76"/>
-      <c r="AC14" s="76"/>
-      <c r="AD14" s="76"/>
-      <c r="AE14" s="80"/>
-      <c r="AF14" s="80"/>
-      <c r="AG14" s="80"/>
+      <c r="T14" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="U14" s="59" t="s">
+        <v>89</v>
+      </c>
+      <c r="V14" s="58" t="s">
+        <v>65</v>
+      </c>
+      <c r="W14" s="57" t="s">
+        <v>90</v>
+      </c>
+      <c r="X14" s="57" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y14" s="58"/>
+      <c r="Z14" s="67" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA14" s="64"/>
+      <c r="AB14" s="64"/>
+      <c r="AC14" s="72"/>
+      <c r="AD14" s="72"/>
+      <c r="AE14" s="72"/>
+      <c r="AF14" s="72"/>
+      <c r="AG14" s="72"/>
+      <c r="AH14" s="72"/>
+      <c r="AI14" s="72"/>
+      <c r="AJ14" s="72"/>
+      <c r="AK14" s="72"/>
+      <c r="AL14" s="72"/>
+      <c r="AM14" s="72"/>
+      <c r="AN14" s="72"/>
+      <c r="AO14" s="72"/>
+      <c r="AP14" s="72"/>
+      <c r="AQ14" s="72"/>
+      <c r="AR14" s="72"/>
+      <c r="AS14" s="72"/>
+      <c r="AT14" s="72"/>
+      <c r="AU14" s="72"/>
     </row>
-    <row r="15" spans="1:33">
+    <row r="15" ht="49.5" spans="1:47">
       <c r="A15" s="20"/>
       <c r="B15" s="21"/>
       <c r="C15" s="22"/>
@@ -2594,159 +3674,227 @@
         <v>36845</v>
       </c>
       <c r="H15" s="22" t="s">
-        <v>42</v>
+        <v>92</v>
       </c>
       <c r="I15" s="22" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="J15" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="K15" s="43">
+        <v>41</v>
+      </c>
+      <c r="K15" s="29">
         <v>0.8295</v>
       </c>
-      <c r="L15" s="43">
+      <c r="L15" s="29">
         <v>0.8155</v>
       </c>
-      <c r="M15" s="50">
+      <c r="M15" s="34">
         <v>1</v>
       </c>
       <c r="N15" s="21">
         <v>36847</v>
       </c>
-      <c r="O15" s="43">
+      <c r="O15" s="29">
         <v>0.8155</v>
       </c>
-      <c r="P15" s="51">
+      <c r="P15" s="35">
         <v>1</v>
       </c>
-      <c r="Q15" s="65">
+      <c r="Q15" s="43">
         <v>0.0179</v>
       </c>
-      <c r="R15" s="66" t="s">
-        <v>41</v>
-      </c>
-      <c r="S15" s="66">
+      <c r="R15" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="S15" s="45">
         <v>-1</v>
       </c>
-      <c r="T15" s="67"/>
-      <c r="U15" s="76"/>
-      <c r="V15" s="76"/>
-      <c r="W15" s="76"/>
-      <c r="X15" s="76"/>
-      <c r="Y15" s="76"/>
-      <c r="Z15" s="76"/>
-      <c r="AA15" s="76"/>
-      <c r="AB15" s="76"/>
-      <c r="AC15" s="76"/>
-      <c r="AD15" s="76"/>
-      <c r="AE15" s="80"/>
-      <c r="AF15" s="80"/>
-      <c r="AG15" s="80"/>
+      <c r="T15" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="U15" s="56" t="s">
+        <v>93</v>
+      </c>
+      <c r="V15" s="57" t="s">
+        <v>35</v>
+      </c>
+      <c r="W15" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="X15" s="57" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y15" s="58"/>
+      <c r="Z15" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA15" s="64"/>
+      <c r="AB15" s="64"/>
+      <c r="AC15" s="72"/>
+      <c r="AD15" s="72"/>
+      <c r="AE15" s="72"/>
+      <c r="AF15" s="72"/>
+      <c r="AG15" s="72"/>
+      <c r="AH15" s="72"/>
+      <c r="AI15" s="72"/>
+      <c r="AJ15" s="72"/>
+      <c r="AK15" s="72"/>
+      <c r="AL15" s="72"/>
+      <c r="AM15" s="72"/>
+      <c r="AN15" s="72"/>
+      <c r="AO15" s="72"/>
+      <c r="AP15" s="72"/>
+      <c r="AQ15" s="72"/>
+      <c r="AR15" s="72"/>
+      <c r="AS15" s="72"/>
+      <c r="AT15" s="72"/>
+      <c r="AU15" s="72"/>
     </row>
-    <row r="16" ht="15.75" spans="1:33">
+    <row r="16" ht="50.25" spans="1:47">
       <c r="A16" s="20"/>
       <c r="B16" s="21"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
-      <c r="F16" s="35">
+      <c r="F16" s="20">
         <v>15</v>
       </c>
-      <c r="G16" s="36">
+      <c r="G16" s="21">
         <v>36864</v>
       </c>
-      <c r="H16" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="I16" s="37" t="s">
-        <v>44</v>
+      <c r="H16" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="I16" s="22" t="s">
+        <v>98</v>
       </c>
       <c r="J16" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="K16" s="43">
+      <c r="K16" s="29">
         <v>0.8625</v>
       </c>
-      <c r="L16" s="43">
+      <c r="L16" s="29">
         <v>0.8765</v>
       </c>
-      <c r="M16" s="50">
+      <c r="M16" s="34">
         <v>1</v>
       </c>
       <c r="N16" s="21">
         <v>36866</v>
       </c>
-      <c r="O16" s="43">
+      <c r="O16" s="29">
         <v>0.8765</v>
       </c>
-      <c r="P16" s="51">
+      <c r="P16" s="35">
         <v>1</v>
       </c>
-      <c r="Q16" s="65">
+      <c r="Q16" s="43">
         <v>0.0172</v>
       </c>
-      <c r="R16" s="66">
+      <c r="R16" s="44">
         <v>2.7</v>
       </c>
-      <c r="S16" s="66">
+      <c r="S16" s="45">
         <v>-1</v>
       </c>
-      <c r="T16" s="67"/>
-      <c r="U16" s="76"/>
-      <c r="V16" s="76"/>
-      <c r="W16" s="76"/>
-      <c r="X16" s="76"/>
-      <c r="Y16" s="76"/>
-      <c r="Z16" s="76"/>
-      <c r="AA16" s="76"/>
-      <c r="AB16" s="76"/>
-      <c r="AC16" s="76"/>
-      <c r="AD16" s="76"/>
-      <c r="AE16" s="80"/>
-      <c r="AF16" s="80"/>
-      <c r="AG16" s="80"/>
+      <c r="T16" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="U16" s="56" t="s">
+        <v>99</v>
+      </c>
+      <c r="V16" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="W16" s="57" t="s">
+        <v>101</v>
+      </c>
+      <c r="X16" s="58" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y16" s="58"/>
+      <c r="Z16" s="70" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA16" s="64"/>
+      <c r="AB16" s="64"/>
+      <c r="AC16" s="72"/>
+      <c r="AD16" s="72"/>
+      <c r="AE16" s="72"/>
+      <c r="AF16" s="72"/>
+      <c r="AG16" s="72"/>
+      <c r="AH16" s="72"/>
+      <c r="AI16" s="72"/>
+      <c r="AJ16" s="72"/>
+      <c r="AK16" s="72"/>
+      <c r="AL16" s="72"/>
+      <c r="AM16" s="72"/>
+      <c r="AN16" s="72"/>
+      <c r="AO16" s="72"/>
+      <c r="AP16" s="72"/>
+      <c r="AQ16" s="72"/>
+      <c r="AR16" s="72"/>
+      <c r="AS16" s="72"/>
+      <c r="AT16" s="72"/>
+      <c r="AU16" s="72"/>
     </row>
-    <row r="17" s="3" customFormat="1" ht="15.75" spans="1:33">
-      <c r="A17" s="23"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="G17" s="24"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="44"/>
-      <c r="L17" s="44"/>
-      <c r="M17" s="52"/>
-      <c r="N17" s="24"/>
-      <c r="O17" s="44"/>
-      <c r="P17" s="53"/>
-      <c r="Q17" s="69">
+    <row r="17" s="1" customFormat="1" ht="15.75" spans="1:47">
+      <c r="A17" s="14"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="15"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="31"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="27"/>
+      <c r="P17" s="31"/>
+      <c r="Q17" s="50">
         <v>-0.1069</v>
       </c>
-      <c r="R17" s="70"/>
-      <c r="S17" s="70"/>
-      <c r="T17" s="71">
+      <c r="R17" s="37"/>
+      <c r="S17" s="37">
+        <v>0.54</v>
+      </c>
+      <c r="T17" s="51">
         <v>0.4</v>
       </c>
-      <c r="U17" s="77"/>
-      <c r="V17" s="77"/>
-      <c r="W17" s="77"/>
-      <c r="X17" s="77"/>
-      <c r="Y17" s="77"/>
-      <c r="Z17" s="77"/>
-      <c r="AA17" s="77"/>
-      <c r="AB17" s="77"/>
-      <c r="AC17" s="77"/>
-      <c r="AD17" s="77"/>
-      <c r="AE17" s="82"/>
-      <c r="AF17" s="82"/>
-      <c r="AG17" s="82"/>
+      <c r="U17" s="52"/>
+      <c r="V17" s="52"/>
+      <c r="W17" s="52"/>
+      <c r="X17" s="52"/>
+      <c r="Y17" s="52"/>
+      <c r="Z17" s="71"/>
+      <c r="AA17" s="62"/>
+      <c r="AB17" s="62"/>
+      <c r="AC17" s="62"/>
+      <c r="AD17" s="62"/>
+      <c r="AE17" s="62"/>
+      <c r="AF17" s="62"/>
+      <c r="AG17" s="62"/>
+      <c r="AH17" s="62"/>
+      <c r="AI17" s="62"/>
+      <c r="AJ17" s="62"/>
+      <c r="AK17" s="62"/>
+      <c r="AL17" s="62"/>
+      <c r="AM17" s="62"/>
+      <c r="AN17" s="62"/>
+      <c r="AO17" s="62"/>
+      <c r="AP17" s="62"/>
+      <c r="AQ17" s="62"/>
+      <c r="AR17" s="62"/>
+      <c r="AS17" s="62"/>
+      <c r="AT17" s="62"/>
+      <c r="AU17" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>